<commit_message>
added DTOs and other classes
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0A23F7-7A1B-43B2-8362-50766F4C47C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0341CDA5-1420-4032-89ED-FB6B8F20B212}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -40,14 +40,52 @@
   </si>
   <si>
     <t>Updating Routing Mechanism</t>
+  </si>
+  <si>
+    <t>Different Service for different model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change name of  namespaces </t>
+  </si>
+  <si>
+    <t>Extensions</t>
+  </si>
+  <si>
+    <t>Model Object  - DTO Object</t>
+  </si>
+  <si>
+    <t>Request Model Object  - Model Object</t>
+  </si>
+  <si>
+    <t>Model Class extra functionality</t>
+  </si>
+  <si>
+    <t>Implement and understand pagination classes</t>
+  </si>
+  <si>
+    <t>Tweet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like count </t>
+  </si>
+  <si>
+    <t>Dislike count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:B7"/>
+  <dimension ref="B3:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +453,58 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tried authentication tokens but not working
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266F8249-648F-4699-8EE3-6B37D3AAE58C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C80D28-E601-435F-BFE8-5A226CF221A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Change all ToDto Method to add Key attribute also</t>
+  </si>
+  <si>
+    <t>Read about  Owin middleware</t>
+  </si>
+  <si>
+    <t>Implement membership Service, CryptoService and everything for authentication and users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete membership and User Services and Managers </t>
   </si>
 </sst>
 </file>
@@ -433,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:B25"/>
+  <dimension ref="B3:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,6 +520,21 @@
         <v>13</v>
       </c>
     </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
verified token and get the key of the logged in user thtough token
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C80D28-E601-435F-BFE8-5A226CF221A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4940817-443B-43DD-B8E0-57E9EC40B98A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">Complete membership and User Services and Managers </t>
+  </si>
+  <si>
+    <t>Validate Token</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:B31"/>
+  <dimension ref="B3:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,6 +538,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
user registeration and login completed with login except validation profile image
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4940817-443B-43DD-B8E0-57E9EC40B98A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD8263-2640-4D12-829E-CB1F8F781405}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -85,6 +85,30 @@
   </si>
   <si>
     <t>Validate Token</t>
+  </si>
+  <si>
+    <t>Make Constructor of Entities for empty collections of relations</t>
+  </si>
+  <si>
+    <t>Learn about Reqgular Expressions</t>
+  </si>
+  <si>
+    <t>Make custom Data Annotation attribute for Image Jpg/PNG format</t>
+  </si>
+  <si>
+    <t>Give validation Error Messages to all Entities</t>
+  </si>
+  <si>
+    <t>Solve Profile Image Dat Issue</t>
+  </si>
+  <si>
+    <t>Error Code while registeration if error comes , don’t pass empty userDto</t>
+  </si>
+  <si>
+    <t>Truncate spaces from starting and ending before saving in database or checkit from frontend while sending it to server</t>
+  </si>
+  <si>
+    <t>Validation for image jpg/png</t>
   </si>
 </sst>
 </file>
@@ -445,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:B33"/>
+  <dimension ref="B3:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,6 +567,46 @@
         <v>17</v>
       </c>
     </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tried adding and fetching user followers and followees
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FD8263-2640-4D12-829E-CB1F8F781405}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE91E7E-FD9D-4CAA-87D9-8E0B1CFA1E2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -109,13 +109,46 @@
   </si>
   <si>
     <t>Validation for image jpg/png</t>
+  </si>
+  <si>
+    <t>Get the followers of a person</t>
+  </si>
+  <si>
+    <t>Get the followings of the person</t>
+  </si>
+  <si>
+    <t>Give follow functionality</t>
+  </si>
+  <si>
+    <t>Give unfollow functionality</t>
+  </si>
+  <si>
+    <t>Give functionality to get the tweets of a person</t>
+  </si>
+  <si>
+    <t>How to extension attributes to a class in c#</t>
+  </si>
+  <si>
+    <t>Give Tweet Adding Functionality</t>
+  </si>
+  <si>
+    <t>Add username functionality</t>
+  </si>
+  <si>
+    <t>While getting followersand unautorized , pass unauthorized and not bad request</t>
+  </si>
+  <si>
+    <t>Make FollowersDto</t>
+  </si>
+  <si>
+    <t>make FolloweesDto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +160,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,9 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:B49"/>
+  <dimension ref="B3:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,9 +644,112 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create new Tweet functionality with their hashtags saved with tweet
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE91E7E-FD9D-4CAA-87D9-8E0B1CFA1E2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A308A9-37D8-47D4-B990-59F3AF20A81B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="43">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -142,6 +142,24 @@
   </si>
   <si>
     <t>make FolloweesDto</t>
+  </si>
+  <si>
+    <t>Make tweets in reverse chronological order</t>
+  </si>
+  <si>
+    <t>Like/Dislike tweet - reaction of tweet</t>
+  </si>
+  <si>
+    <t>Edit/Delete tweet option to the tweet owner</t>
+  </si>
+  <si>
+    <t>Tweet Hashtags and Tweet User handling</t>
+  </si>
+  <si>
+    <t>Duplcate entries in follower table handling put index on entries</t>
+  </si>
+  <si>
+    <t>Hashtags are case insensitive - I think its good</t>
   </si>
 </sst>
 </file>
@@ -511,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:F69"/>
+  <dimension ref="B3:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,20 +693,20 @@
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
@@ -724,12 +742,17 @@
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
       <c r="E61" s="2"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
@@ -737,19 +760,75 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented tweet edit and delete feature
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A308A9-37D8-47D4-B990-59F3AF20A81B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2034F7E-7C16-45D2-AAC8-C6A5ED3B54A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Hashtags are case insensitive - I think its good</t>
+  </si>
+  <si>
+    <t>Recheck GetUserDashboardTweets for Union/AddRange implementation</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:F81"/>
+  <dimension ref="B3:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +779,7 @@
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C71" s="2"/>
@@ -831,6 +834,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
merged API and Webhost into WebAPI for resolving error
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2034F7E-7C16-45D2-AAC8-C6A5ED3B54A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1347274C-879D-4011-A8B7-9CF83B70970C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -163,13 +163,111 @@
   </si>
   <si>
     <t>Recheck GetUserDashboardTweets for Union/AddRange implementation</t>
+  </si>
+  <si>
+    <t>Server Side</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>first complete Authentication part</t>
+  </si>
+  <si>
+    <t>accessing static files css, installing bootstrap</t>
+  </si>
+  <si>
+    <r>
+      <t>making child components and passign data in child component using</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF24292E"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF444D56"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>@input</t>
+    </r>
+  </si>
+  <si>
+    <t>passing info from child to parent using event emitter</t>
+  </si>
+  <si>
+    <t>using template reference variable # to interact with child components</t>
+  </si>
+  <si>
+    <t>removed output emitter and template variable logic</t>
+  </si>
+  <si>
+    <t>angular styling ysung ngClass and ngStyle</t>
+  </si>
+  <si>
+    <t>using first simple service</t>
+  </si>
+  <si>
+    <t>using toastr services</t>
+  </si>
+  <si>
+    <t>correction in toastr- added jquery js in angular.json</t>
+  </si>
+  <si>
+    <t>created routes components</t>
+  </si>
+  <si>
+    <t>used a simple routing</t>
+  </si>
+  <si>
+    <t>accessing route parameters in component</t>
+  </si>
+  <si>
+    <t>created link for routes- routerLink</t>
+  </si>
+  <si>
+    <t>navigation in routes through components functions</t>
+  </si>
+  <si>
+    <t>guarding against route activation using CanActivate</t>
+  </si>
+  <si>
+    <t>guarding against route de-activation using CanDeactivate</t>
+  </si>
+  <si>
+    <t>tried using resolvers but no data is fetched, no error, not working</t>
+  </si>
+  <si>
+    <t>pre-loading data for components using resolvers and route parameters</t>
+  </si>
+  <si>
+    <t>styling active links using routerLinkActive and routerLinkActiveOptions</t>
+  </si>
+  <si>
+    <t>lazy loading feature module and different components</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Create Home Module and Models first</t>
+  </si>
+  <si>
+    <t>Make a user controller t give user details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +290,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF444D56"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -210,16 +336,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,14 +663,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B3:F83"/>
+  <dimension ref="B1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
@@ -839,8 +975,154 @@
         <v>43</v>
       </c>
     </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B86" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B90" r:id="rId1" display="https://github.com/himanshu-uppal/EventsApp/commit/4a849dbaffa78743dcba82fe265cf4b6d3d3761c" xr:uid="{0155BACD-D2EB-4227-97DF-B6D972BB5955}"/>
+    <hyperlink ref="B94" r:id="rId2" display="https://github.com/himanshu-uppal/EventsApp/commit/b959da15aaffc22f0da700d69dd5d6ae99b53994" xr:uid="{D066FD60-7F77-4CA8-9ADD-5D76F498A106}"/>
+    <hyperlink ref="B96" r:id="rId3" display="https://github.com/himanshu-uppal/EventsApp/commit/0ade16512ac6ca3c77ff7b3488f5ebad900b851b" xr:uid="{A45CE2AD-00D2-4678-BAE7-839C48BCB011}"/>
+    <hyperlink ref="B98" r:id="rId4" display="https://github.com/himanshu-uppal/EventsApp/commit/5d9373dc4ed2ab6010eda217c402f1a38a30d0b0" xr:uid="{AEF0123A-73C1-4905-9AB9-96472E8776B3}"/>
+    <hyperlink ref="B100" r:id="rId5" display="https://github.com/himanshu-uppal/EventsApp/commit/75188fae615427a37d8bff0e6b9be331d6a41807" xr:uid="{9F210BFA-DFE4-442A-B5DF-1D4CF7942D8E}"/>
+    <hyperlink ref="B102" r:id="rId6" display="https://github.com/himanshu-uppal/EventsApp/commit/0b5995aeb8e0274fc89695a850f606e27d78bc21" xr:uid="{BCB10871-DB39-48C3-942A-09A0B2C2639F}"/>
+    <hyperlink ref="B104" r:id="rId7" display="https://github.com/himanshu-uppal/EventsApp/commit/c14160aa48c3373c107b5c97cf9996f7d655f5a6" xr:uid="{059D8885-BAF1-41D1-AB90-8883ACCB3115}"/>
+    <hyperlink ref="B106" r:id="rId8" display="https://github.com/himanshu-uppal/EventsApp/commit/6bd9ec3a8368cccb732a6001270948d22db5c043" xr:uid="{F2F250E6-CCF4-4B76-998A-480A9EEBCE5F}"/>
+    <hyperlink ref="B108" r:id="rId9" display="https://github.com/himanshu-uppal/EventsApp/commit/5c5f3a987d2ce05c756594c6dc39625a734cd2b3" xr:uid="{BF3314DF-A6AC-4658-B6BF-84EFD2541CB1}"/>
+    <hyperlink ref="B110" r:id="rId10" display="https://github.com/himanshu-uppal/EventsApp/commit/cea2911a1f210e5b25136815e99c9e4cde00c543" xr:uid="{F050FBFF-69BA-44C0-961B-F9D80EB0C8DA}"/>
+    <hyperlink ref="B112" r:id="rId11" display="https://github.com/himanshu-uppal/EventsApp/commit/ac2da4e61c4256fc7311ad1eb83d77371e3821d2" xr:uid="{804ED8B1-26F4-4D73-9344-82833D7F19E2}"/>
+    <hyperlink ref="B114" r:id="rId12" display="https://github.com/himanshu-uppal/EventsApp/commit/a39e79a0d58c2459cc048482a7867d38a5c189be" xr:uid="{EA79ABE8-F9F1-484A-BFFF-8AEAF918A68A}"/>
+    <hyperlink ref="B116" r:id="rId13" display="https://github.com/himanshu-uppal/EventsApp/commit/f2e5507006ab4217c19afbbb740040ea1ed209cd" xr:uid="{7D796F88-B696-4CD8-BAB2-666281AF98CD}"/>
+    <hyperlink ref="B118" r:id="rId14" display="https://github.com/himanshu-uppal/EventsApp/commit/88e08ce5b1bec2e5db5c949e35aab4589e9af43d" xr:uid="{6F79B857-5003-4F3B-94B7-D8E63E383F1E}"/>
+    <hyperlink ref="B120" r:id="rId15" display="https://github.com/himanshu-uppal/EventsApp/commit/0e93d7a4baadb00ecefb2d200401e72dfc6e29b9" xr:uid="{1EE24675-EDCB-4303-8F2D-533C0AC1F1A5}"/>
+    <hyperlink ref="B122" r:id="rId16" display="https://github.com/himanshu-uppal/EventsApp/commit/05b2604820195dc5631cc1f08ec9509d20203a94" xr:uid="{FA97DC72-6D2E-4612-AF71-7BC8877540DA}"/>
+    <hyperlink ref="B124" r:id="rId17" display="https://github.com/himanshu-uppal/EventsApp/commit/c7cc6663edc19fa5ef52d8088ca11cf7d2e97bf3" xr:uid="{8ABC7648-E1AA-458C-AA05-9BAC17D8556D}"/>
+    <hyperlink ref="B126" r:id="rId18" display="https://github.com/himanshu-uppal/EventsApp/commit/77e140f464ef677f6b594063c7e5c342bd4e1229" xr:uid="{7C63B72D-AFEA-44FB-908F-437BC999D261}"/>
+    <hyperlink ref="B128" r:id="rId19" display="https://github.com/himanshu-uppal/EventsApp/commit/31c97f300b958fc47bc2b8d1d476278b3d2250f2" xr:uid="{5E50781C-CFDD-4D2C-B459-180E1A622819}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed a hell lot of shit
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Assignments\ExitTest\Glitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1347274C-879D-4011-A8B7-9CF83B70970C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BC7D2D-BBEE-4AF0-9B7C-70E794768147}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8988" xr2:uid="{A70599B4-F12C-47C9-B869-23238B21FD51}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Make URI template for all APIs</t>
   </si>
@@ -262,12 +262,60 @@
   <si>
     <t>Make a user controller t give user details</t>
   </si>
+  <si>
+    <t>Make Routes for API defination on Home page</t>
+  </si>
+  <si>
+    <t>home-component.html is called first than home-componentts</t>
+  </si>
+  <si>
+    <t>Take care of capital and smalls semt and received</t>
+  </si>
+  <si>
+    <t>Check the chronological order of tweets on feed page</t>
+  </si>
+  <si>
+    <t>If reply comes as unauthorized , then land on login page</t>
+  </si>
+  <si>
+    <t>Highlight hashtag in a post and make it hyperlink when clicked shows the post of that hashtag</t>
+  </si>
+  <si>
+    <t>put empty body in all post request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compose a Tweet </t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>change all Dto responses to array attributes , count and others</t>
+  </si>
+  <si>
+    <t>put that route annotation before every controller</t>
+  </si>
+  <si>
+    <t>Follow/Unfollow Option</t>
+  </si>
+  <si>
+    <t>Important Tasks</t>
+  </si>
+  <si>
+    <t>Edit a tweet</t>
+  </si>
+  <si>
+    <t>create a tweet</t>
+  </si>
+  <si>
+    <t>Make Create/Edit Tweet TextArea</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +366,22 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -340,7 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -348,6 +412,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -663,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513F3294-7872-42CE-9F6B-784528CEE488}">
-  <dimension ref="B1:F133"/>
+  <dimension ref="B1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,155 +1038,242 @@
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B86" s="4" t="s">
+    <row r="88" spans="2:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B88" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B88" t="s">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B90" s="5" t="s">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B92" s="6" t="s">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="6" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B94" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="5" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B131" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B147" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B149" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B151" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B153" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+      <c r="B157" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C157" s="7"/>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B159" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B160" s="3"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="8"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B165" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B90" r:id="rId1" display="https://github.com/himanshu-uppal/EventsApp/commit/4a849dbaffa78743dcba82fe265cf4b6d3d3761c" xr:uid="{0155BACD-D2EB-4227-97DF-B6D972BB5955}"/>
-    <hyperlink ref="B94" r:id="rId2" display="https://github.com/himanshu-uppal/EventsApp/commit/b959da15aaffc22f0da700d69dd5d6ae99b53994" xr:uid="{D066FD60-7F77-4CA8-9ADD-5D76F498A106}"/>
-    <hyperlink ref="B96" r:id="rId3" display="https://github.com/himanshu-uppal/EventsApp/commit/0ade16512ac6ca3c77ff7b3488f5ebad900b851b" xr:uid="{A45CE2AD-00D2-4678-BAE7-839C48BCB011}"/>
-    <hyperlink ref="B98" r:id="rId4" display="https://github.com/himanshu-uppal/EventsApp/commit/5d9373dc4ed2ab6010eda217c402f1a38a30d0b0" xr:uid="{AEF0123A-73C1-4905-9AB9-96472E8776B3}"/>
-    <hyperlink ref="B100" r:id="rId5" display="https://github.com/himanshu-uppal/EventsApp/commit/75188fae615427a37d8bff0e6b9be331d6a41807" xr:uid="{9F210BFA-DFE4-442A-B5DF-1D4CF7942D8E}"/>
-    <hyperlink ref="B102" r:id="rId6" display="https://github.com/himanshu-uppal/EventsApp/commit/0b5995aeb8e0274fc89695a850f606e27d78bc21" xr:uid="{BCB10871-DB39-48C3-942A-09A0B2C2639F}"/>
-    <hyperlink ref="B104" r:id="rId7" display="https://github.com/himanshu-uppal/EventsApp/commit/c14160aa48c3373c107b5c97cf9996f7d655f5a6" xr:uid="{059D8885-BAF1-41D1-AB90-8883ACCB3115}"/>
-    <hyperlink ref="B106" r:id="rId8" display="https://github.com/himanshu-uppal/EventsApp/commit/6bd9ec3a8368cccb732a6001270948d22db5c043" xr:uid="{F2F250E6-CCF4-4B76-998A-480A9EEBCE5F}"/>
-    <hyperlink ref="B108" r:id="rId9" display="https://github.com/himanshu-uppal/EventsApp/commit/5c5f3a987d2ce05c756594c6dc39625a734cd2b3" xr:uid="{BF3314DF-A6AC-4658-B6BF-84EFD2541CB1}"/>
-    <hyperlink ref="B110" r:id="rId10" display="https://github.com/himanshu-uppal/EventsApp/commit/cea2911a1f210e5b25136815e99c9e4cde00c543" xr:uid="{F050FBFF-69BA-44C0-961B-F9D80EB0C8DA}"/>
-    <hyperlink ref="B112" r:id="rId11" display="https://github.com/himanshu-uppal/EventsApp/commit/ac2da4e61c4256fc7311ad1eb83d77371e3821d2" xr:uid="{804ED8B1-26F4-4D73-9344-82833D7F19E2}"/>
-    <hyperlink ref="B114" r:id="rId12" display="https://github.com/himanshu-uppal/EventsApp/commit/a39e79a0d58c2459cc048482a7867d38a5c189be" xr:uid="{EA79ABE8-F9F1-484A-BFFF-8AEAF918A68A}"/>
-    <hyperlink ref="B116" r:id="rId13" display="https://github.com/himanshu-uppal/EventsApp/commit/f2e5507006ab4217c19afbbb740040ea1ed209cd" xr:uid="{7D796F88-B696-4CD8-BAB2-666281AF98CD}"/>
-    <hyperlink ref="B118" r:id="rId14" display="https://github.com/himanshu-uppal/EventsApp/commit/88e08ce5b1bec2e5db5c949e35aab4589e9af43d" xr:uid="{6F79B857-5003-4F3B-94B7-D8E63E383F1E}"/>
-    <hyperlink ref="B120" r:id="rId15" display="https://github.com/himanshu-uppal/EventsApp/commit/0e93d7a4baadb00ecefb2d200401e72dfc6e29b9" xr:uid="{1EE24675-EDCB-4303-8F2D-533C0AC1F1A5}"/>
-    <hyperlink ref="B122" r:id="rId16" display="https://github.com/himanshu-uppal/EventsApp/commit/05b2604820195dc5631cc1f08ec9509d20203a94" xr:uid="{FA97DC72-6D2E-4612-AF71-7BC8877540DA}"/>
-    <hyperlink ref="B124" r:id="rId17" display="https://github.com/himanshu-uppal/EventsApp/commit/c7cc6663edc19fa5ef52d8088ca11cf7d2e97bf3" xr:uid="{8ABC7648-E1AA-458C-AA05-9BAC17D8556D}"/>
-    <hyperlink ref="B126" r:id="rId18" display="https://github.com/himanshu-uppal/EventsApp/commit/77e140f464ef677f6b594063c7e5c342bd4e1229" xr:uid="{7C63B72D-AFEA-44FB-908F-437BC999D261}"/>
-    <hyperlink ref="B128" r:id="rId19" display="https://github.com/himanshu-uppal/EventsApp/commit/31c97f300b958fc47bc2b8d1d476278b3d2250f2" xr:uid="{5E50781C-CFDD-4D2C-B459-180E1A622819}"/>
+    <hyperlink ref="B92" r:id="rId1" display="https://github.com/himanshu-uppal/EventsApp/commit/4a849dbaffa78743dcba82fe265cf4b6d3d3761c" xr:uid="{0155BACD-D2EB-4227-97DF-B6D972BB5955}"/>
+    <hyperlink ref="B96" r:id="rId2" display="https://github.com/himanshu-uppal/EventsApp/commit/b959da15aaffc22f0da700d69dd5d6ae99b53994" xr:uid="{D066FD60-7F77-4CA8-9ADD-5D76F498A106}"/>
+    <hyperlink ref="B98" r:id="rId3" display="https://github.com/himanshu-uppal/EventsApp/commit/0ade16512ac6ca3c77ff7b3488f5ebad900b851b" xr:uid="{A45CE2AD-00D2-4678-BAE7-839C48BCB011}"/>
+    <hyperlink ref="B100" r:id="rId4" display="https://github.com/himanshu-uppal/EventsApp/commit/5d9373dc4ed2ab6010eda217c402f1a38a30d0b0" xr:uid="{AEF0123A-73C1-4905-9AB9-96472E8776B3}"/>
+    <hyperlink ref="B102" r:id="rId5" display="https://github.com/himanshu-uppal/EventsApp/commit/75188fae615427a37d8bff0e6b9be331d6a41807" xr:uid="{9F210BFA-DFE4-442A-B5DF-1D4CF7942D8E}"/>
+    <hyperlink ref="B104" r:id="rId6" display="https://github.com/himanshu-uppal/EventsApp/commit/0b5995aeb8e0274fc89695a850f606e27d78bc21" xr:uid="{BCB10871-DB39-48C3-942A-09A0B2C2639F}"/>
+    <hyperlink ref="B106" r:id="rId7" display="https://github.com/himanshu-uppal/EventsApp/commit/c14160aa48c3373c107b5c97cf9996f7d655f5a6" xr:uid="{059D8885-BAF1-41D1-AB90-8883ACCB3115}"/>
+    <hyperlink ref="B108" r:id="rId8" display="https://github.com/himanshu-uppal/EventsApp/commit/6bd9ec3a8368cccb732a6001270948d22db5c043" xr:uid="{F2F250E6-CCF4-4B76-998A-480A9EEBCE5F}"/>
+    <hyperlink ref="B110" r:id="rId9" display="https://github.com/himanshu-uppal/EventsApp/commit/5c5f3a987d2ce05c756594c6dc39625a734cd2b3" xr:uid="{BF3314DF-A6AC-4658-B6BF-84EFD2541CB1}"/>
+    <hyperlink ref="B112" r:id="rId10" display="https://github.com/himanshu-uppal/EventsApp/commit/cea2911a1f210e5b25136815e99c9e4cde00c543" xr:uid="{F050FBFF-69BA-44C0-961B-F9D80EB0C8DA}"/>
+    <hyperlink ref="B114" r:id="rId11" display="https://github.com/himanshu-uppal/EventsApp/commit/ac2da4e61c4256fc7311ad1eb83d77371e3821d2" xr:uid="{804ED8B1-26F4-4D73-9344-82833D7F19E2}"/>
+    <hyperlink ref="B116" r:id="rId12" display="https://github.com/himanshu-uppal/EventsApp/commit/a39e79a0d58c2459cc048482a7867d38a5c189be" xr:uid="{EA79ABE8-F9F1-484A-BFFF-8AEAF918A68A}"/>
+    <hyperlink ref="B118" r:id="rId13" display="https://github.com/himanshu-uppal/EventsApp/commit/f2e5507006ab4217c19afbbb740040ea1ed209cd" xr:uid="{7D796F88-B696-4CD8-BAB2-666281AF98CD}"/>
+    <hyperlink ref="B120" r:id="rId14" display="https://github.com/himanshu-uppal/EventsApp/commit/88e08ce5b1bec2e5db5c949e35aab4589e9af43d" xr:uid="{6F79B857-5003-4F3B-94B7-D8E63E383F1E}"/>
+    <hyperlink ref="B122" r:id="rId15" display="https://github.com/himanshu-uppal/EventsApp/commit/0e93d7a4baadb00ecefb2d200401e72dfc6e29b9" xr:uid="{1EE24675-EDCB-4303-8F2D-533C0AC1F1A5}"/>
+    <hyperlink ref="B124" r:id="rId16" display="https://github.com/himanshu-uppal/EventsApp/commit/05b2604820195dc5631cc1f08ec9509d20203a94" xr:uid="{FA97DC72-6D2E-4612-AF71-7BC8877540DA}"/>
+    <hyperlink ref="B126" r:id="rId17" display="https://github.com/himanshu-uppal/EventsApp/commit/c7cc6663edc19fa5ef52d8088ca11cf7d2e97bf3" xr:uid="{8ABC7648-E1AA-458C-AA05-9BAC17D8556D}"/>
+    <hyperlink ref="B128" r:id="rId18" display="https://github.com/himanshu-uppal/EventsApp/commit/77e140f464ef677f6b594063c7e5c342bd4e1229" xr:uid="{7C63B72D-AFEA-44FB-908F-437BC999D261}"/>
+    <hyperlink ref="B130" r:id="rId19" display="https://github.com/himanshu-uppal/EventsApp/commit/31c97f300b958fc47bc2b8d1d476278b3d2250f2" xr:uid="{5E50781C-CFDD-4D2C-B459-180E1A622819}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>

</xml_diff>